<commit_message>
Updating XLSX sheets with formatting
</commit_message>
<xml_diff>
--- a/stat_tests/ya_block_data.xlsx
+++ b/stat_tests/ya_block_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasminebassil/Documents/Emory/3_Research/Projects/NavAging_Paper/stat_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2F98644B-D74D-E840-B5F4-192142A14458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8AB8DD72-0D29-8948-BCB3-A946F0724C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ya_block_data" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -685,6 +685,16 @@
   <dxfs count="6">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -710,16 +720,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1052,17 +1052,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1170,7 +1170,7 @@
       <c r="F4">
         <v>2.0900767056927299</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>9.2730895718621295E-2</v>
       </c>
       <c r="H4" s="1">
@@ -1260,7 +1260,7 @@
       <c r="F7">
         <v>1.4921599372169101</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>0.29539059051808902</v>
       </c>
       <c r="H7" s="1">
@@ -1440,7 +1440,7 @@
       <c r="F13">
         <v>1.92090847726453</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>0.13365600971448399</v>
       </c>
       <c r="H13" s="1">
@@ -1530,7 +1530,7 @@
       <c r="F16">
         <v>3.0590800616281602</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>6.5508228168620298E-3</v>
       </c>
       <c r="H16" s="1">
@@ -1710,7 +1710,7 @@
       <c r="F22">
         <v>1.4467111884772199</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>0.31766812608786699</v>
       </c>
       <c r="H22" s="1">
@@ -1723,16 +1723,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
       <formula>0.05</formula>
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>0.01</formula>
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0.001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>0.01</formula>
+      <formula>0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+      <formula>0.05</formula>
+      <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>